<commit_message>
Style Loading and Updating in Edit mode - Color Scheme Them All In progress
</commit_message>
<xml_diff>
--- a/Tests/TestFiles/basic_test.xlsx
+++ b/Tests/TestFiles/basic_test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dravia Vemal\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dravia Vemal\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{57A8591D-8FC6-46EF-B9E0-9D3BE6E317F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15FB91D3-7628-4A80-8E9B-5609B8668AF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{D55DE239-15DF-4A49-97E5-A2E7014A78CA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{D55DE239-15DF-4A49-97E5-A2E7014A78CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Test File</t>
   </si>
@@ -90,12 +90,58 @@
   <si>
     <t>cat5</t>
   </si>
+  <si>
+    <t>Top</t>
+  </si>
+  <si>
+    <t>Center</t>
+  </si>
+  <si>
+    <t>Bottom</t>
+  </si>
+  <si>
+    <t>Left</t>
+  </si>
+  <si>
+    <t>Right</t>
+  </si>
+  <si>
+    <t>Bold</t>
+  </si>
+  <si>
+    <t>Italic</t>
+  </si>
+  <si>
+    <t>Wrap Text</t>
+  </si>
+  <si>
+    <t>Font size</t>
+  </si>
+  <si>
+    <t>Font Family</t>
+  </si>
+  <si>
+    <t>background color</t>
+  </si>
+  <si>
+    <t>foreground color</t>
+  </si>
+  <si>
+    <t>underline</t>
+  </si>
+  <si>
+    <t>Double Underline</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,13 +155,78 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Book Antiqua"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u val="double"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -127,14 +238,44 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2176,7 +2317,7 @@
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2680,18 +2821,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF7BEDD7-1ADD-41DF-8086-36FAD0D7EED2}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:V20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Y19" sqref="Y19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="20" max="20" width="10.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -2699,7 +2843,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -2707,19 +2851,84 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>2</v>
       </c>
+      <c r="T6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="U6" s="9" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>3</v>
+      </c>
+      <c r="T7" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="U7" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="T8" t="s">
+        <v>12</v>
+      </c>
+      <c r="U8" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+      <c r="T10" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="U10" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="V10" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="T12" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="T13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="V13" s="14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="T15" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="V15" s="15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="T16" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="20:22" x14ac:dyDescent="0.25">
+      <c r="T20" s="16">
+        <v>10000</v>
+      </c>
+      <c r="V20" s="17">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2733,7 +2942,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{653FCBA5-C94D-4AE4-B591-50B1B975489C}">
   <dimension ref="B5:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Excel Merge Cell Update
</commit_message>
<xml_diff>
--- a/Tests/TestFiles/basic_test.xlsx
+++ b/Tests/TestFiles/basic_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\draviavemal\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{66001197-5982-4B6B-8E40-E5AEB0D41969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4F0B207-BBD4-4410-85C1-8250F429FEC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2475" yWindow="510" windowWidth="28800" windowHeight="15345" xr2:uid="{55A69094-CFF0-4A24-937F-3F8966A07938}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{55A69094-CFF0-4A24-937F-3F8966A07938}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Different Family</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>Neutral</t>
+  </si>
+  <si>
+    <t>Merge Cell</t>
   </si>
 </sst>
 </file>
@@ -113,7 +116,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="&quot;₹&quot;\ #,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;₹&quot;\ #,##0.00"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -299,7 +302,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -315,7 +318,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -338,6 +341,9 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -655,10 +661,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F3B5DA4-290A-42B9-8806-349169E1CF0E}">
-  <dimension ref="B2:J23"/>
+  <dimension ref="B2:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -780,7 +786,27 @@
         <v>9</v>
       </c>
     </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E25" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E26" s="26"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="26"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="26"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E25:G27"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>